<commit_message>
LV Scan - build plate w tape
</commit_message>
<xml_diff>
--- a/system_development/Orichalcum/v0.2/Software_design/v2-cover-control/VIBROMETER SCAN SETTINGS.xlsx
+++ b/system_development/Orichalcum/v0.2/Software_design/v2-cover-control/VIBROMETER SCAN SETTINGS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\In-situ-monitoring-of-powder-bed-fusion-additive-manufacturing\system_development\Orichalcum\v0.2\Software_design\v2-cover-control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5539441-6A87-4F5A-B9F3-AC7AB791E151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80D26A8-021C-4F41-BFEE-7767015D84F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
   <si>
     <t>Receiver</t>
   </si>
@@ -259,12 +259,6 @@
     <t>Test Scan 1</t>
   </si>
   <si>
-    <t>Trigger Source</t>
-  </si>
-  <si>
-    <t>Resource Name</t>
-  </si>
-  <si>
     <t>PXI1Slot2</t>
   </si>
   <si>
@@ -314,13 +308,62 @@
   </si>
   <si>
     <t>Test Scan 3</t>
+  </si>
+  <si>
+    <t>(HTML generated, data folder overwritten)</t>
+  </si>
+  <si>
+    <t>Test Scan 4</t>
+  </si>
+  <si>
+    <t>build plate with square tape</t>
+  </si>
+  <si>
+    <t>Test Scan 5</t>
+  </si>
+  <si>
+    <t>tape square on build plate</t>
+  </si>
+  <si>
+    <t>averages</t>
+  </si>
+  <si>
+    <t>25mm^2</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>noisey/didn't run</t>
+  </si>
+  <si>
+    <t>20k</t>
+  </si>
+  <si>
+    <t>Test Scan 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample
+Rate </t>
+  </si>
+  <si>
+    <t>Min Record
+Length</t>
+  </si>
+  <si>
+    <t>Resource
+Name</t>
+  </si>
+  <si>
+    <t>Trigger
+Source</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -369,6 +412,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -429,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,7 +503,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -488,6 +535,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,165 +819,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A5D31-C167-4FC4-94A5-027E9DD85F49}">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.21875" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="11" width="8.109375" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3"/>
     </row>
-    <row r="4" spans="2:12" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>61</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="D4" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5">
+        <v>50</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>-700</v>
+      </c>
+      <c r="K5">
+        <v>500</v>
+      </c>
+      <c r="L5">
+        <v>14</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F5">
+      <c r="E6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6">
+        <v>60</v>
+      </c>
+      <c r="I6">
+        <v>60</v>
+      </c>
+      <c r="J6">
+        <v>-900</v>
+      </c>
+      <c r="K6">
+        <v>200</v>
+      </c>
+      <c r="L6">
+        <v>15</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7">
         <v>50</v>
       </c>
-      <c r="G5">
+      <c r="I7">
         <v>50</v>
       </c>
-      <c r="H5">
+      <c r="J7">
+        <v>-1000</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="O7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6">
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>50</v>
+      </c>
+      <c r="J8">
         <v>-700</v>
       </c>
-      <c r="I5">
-        <v>500</v>
-      </c>
-      <c r="J5">
+      <c r="K8">
+        <v>300</v>
+      </c>
+      <c r="L8">
         <v>14</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="N8" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F6">
-        <v>60</v>
-      </c>
-      <c r="G6">
-        <v>60</v>
-      </c>
-      <c r="H6">
-        <v>-900</v>
-      </c>
-      <c r="I6">
-        <v>200</v>
-      </c>
-      <c r="J6">
-        <v>15</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="E9" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G9" s="6">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="6">
+        <v>25</v>
+      </c>
+      <c r="I9">
+        <v>25</v>
+      </c>
+      <c r="J9">
+        <v>-380</v>
+      </c>
+      <c r="K9">
+        <v>600</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>32</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F7">
-        <v>50</v>
-      </c>
-      <c r="G7">
-        <v>50</v>
-      </c>
-      <c r="H7">
-        <v>-1000</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>20</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>87</v>
+      <c r="E10" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -938,7 +1107,7 @@
   <dimension ref="B1:I1001"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -958,14 +1127,14 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="F2" s="19" t="s">
+      <c r="D2" s="21"/>
+      <c r="F2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
@@ -1042,10 +1211,10 @@
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="20"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
@@ -1093,10 +1262,10 @@
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="22"/>
+      <c r="C13" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
@@ -1130,14 +1299,14 @@
       <c r="D16" s="3">
         <v>1</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="17" t="s">
+      <c r="G16" s="15"/>
+      <c r="H16" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="18"/>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
@@ -1237,7 +1406,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -1261,7 +1430,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="4" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1449,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
+      <c r="B24" s="13"/>
       <c r="C24" s="4" t="s">
         <v>35</v>
       </c>
@@ -1289,7 +1458,7 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
+      <c r="B25" s="13"/>
       <c r="C25" s="4" t="s">
         <v>36</v>
       </c>
@@ -1298,7 +1467,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="4" t="s">
         <v>37</v>
       </c>
@@ -1315,17 +1484,17 @@
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D29" s="13"/>
+      <c r="C29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="12"/>
       <c r="F29" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C30" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -1333,7 +1502,7 @@
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
@@ -1344,7 +1513,7 @@
         <v>66</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
@@ -1352,7 +1521,7 @@
         <v>67</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
@@ -1367,19 +1536,19 @@
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="13"/>
+      <c r="C36" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>